<commit_message>
Agregamos detalle de los rangos intercuartilicos
</commit_message>
<xml_diff>
--- a/frecuencias_fallecidos.xlsx
+++ b/frecuencias_fallecidos.xlsx
@@ -370,7 +370,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>variable</t>
+          <t>Enfermedad</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -388,7 +388,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>copd</t>
+          <t>EPOC</t>
         </is>
       </c>
       <c r="D2">
@@ -404,7 +404,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>obesity</t>
+          <t>Obesidad</t>
         </is>
       </c>
       <c r="D3">
@@ -420,7 +420,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>renal_disease</t>
+          <t>Enfermedad Renal</t>
         </is>
       </c>
       <c r="D4">
@@ -436,7 +436,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>hypertension</t>
+          <t>Hipertensión</t>
         </is>
       </c>
       <c r="D5">
@@ -452,7 +452,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ihd</t>
+          <t>Cardiopatía Isquémica</t>
         </is>
       </c>
       <c r="D6">
@@ -468,7 +468,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>pvd</t>
+          <t>Enfermedad Vascular Periférica</t>
         </is>
       </c>
       <c r="D7">
@@ -484,7 +484,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>valvular_disease</t>
+          <t>Enfermedad Valvular Cardíaca</t>
         </is>
       </c>
       <c r="D8">
@@ -500,7 +500,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>Cáncer</t>
         </is>
       </c>
       <c r="D9">
@@ -516,7 +516,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>pneumonia</t>
+          <t>Neumonía</t>
         </is>
       </c>
       <c r="D10">
@@ -532,7 +532,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>stroke</t>
+          <t>ACV</t>
         </is>
       </c>
       <c r="D11">

</xml_diff>